<commit_message>
Add animations on vetrina
</commit_message>
<xml_diff>
--- a/a-lan00/datiPC/PC.xlsx
+++ b/a-lan00/datiPC/PC.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Assembler\a-lan00\datiPC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Foglio1" sheetId="1" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t xml:space="preserve">PC
 </t>
@@ -72,15 +80,6 @@
     <t>Win</t>
   </si>
   <si>
-    <t>Sahara P35</t>
-  </si>
-  <si>
-    <t>Cooler Master MasterLiquid</t>
-  </si>
-  <si>
-    <t>Cooler Master MasterWatt 650</t>
-  </si>
-  <si>
     <t>Intel Core i5 9600K</t>
   </si>
   <si>
@@ -148,25 +147,88 @@
   </si>
   <si>
     <t>Cooler Master MasterWatt 750 80 Brone plus</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B01GCWQ2MY/?tag=config46-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperX Predator DDR4 HX430C15PB3K2/8 Kit 8 GB (2 x 4 GB), 3000 MHz, DDR4 CL15 DIMM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zotac ZT-T16500F-10L scheda video GeForce GTX 1650 4 GB GDDR5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SanDisk Plus SSD Unità a Stato Solido 240 GB, Velocità di Lettura fino a 530 MB/s, 2,5", Sata III </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corsair Carbide 100R Case da Gaming, Mid-Tower ATX, con Finestra, Nero </t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B07P871J57/?tag=config46-21</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B07W8389W5/?tag=config46-21</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B076JG8FS1/?tag=config46-21</t>
+  </si>
+  <si>
+    <t>564.56</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B077D9YWHT/?tag=config46-21</t>
+  </si>
+  <si>
+    <t>553.36</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B07WC8QVCB/?tag=config46-21</t>
+  </si>
+  <si>
+    <t>Seagate 1TB / Crucial 120Gb</t>
+  </si>
+  <si>
+    <t>https://www.amazon.it/dp/B0711QH8ZS/?tag=config46-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,39 +236,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -396,25 +468,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="16.57"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="16.71"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,21 +532,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>17</v>
@@ -477,28 +554,28 @@
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1">
-        <v>925.0</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
@@ -507,207 +584,234 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1252</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1">
-        <v>1252.0</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J4" s="1">
-        <v>1788.0</v>
+        <v>1788</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
+      <c r="F5" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" s="1">
-        <v>810.0</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1263</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1263.0</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2581</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="1">
-        <v>2581.0</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
         <v>44</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="1">
+        <v>691</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="F2"/>
-    <hyperlink r:id="rId4" ref="G2"/>
-    <hyperlink r:id="rId5" ref="I2"/>
-    <hyperlink r:id="rId6" ref="L2"/>
-    <hyperlink r:id="rId7" ref="M2"/>
-    <hyperlink r:id="rId8" ref="C3"/>
-    <hyperlink r:id="rId9" ref="E3"/>
-    <hyperlink r:id="rId10" ref="F3"/>
-    <hyperlink r:id="rId11" ref="G3"/>
-    <hyperlink r:id="rId12" ref="I3"/>
-    <hyperlink r:id="rId13" ref="L3"/>
-    <hyperlink r:id="rId14" ref="M3"/>
-    <hyperlink r:id="rId15" ref="C4"/>
-    <hyperlink r:id="rId16" ref="E4"/>
-    <hyperlink r:id="rId17" ref="F4"/>
-    <hyperlink r:id="rId18" ref="G4"/>
-    <hyperlink r:id="rId19" ref="I4"/>
-    <hyperlink r:id="rId20" ref="L4"/>
-    <hyperlink r:id="rId21" ref="M4"/>
-    <hyperlink r:id="rId22" ref="C5"/>
-    <hyperlink r:id="rId23" ref="E5"/>
-    <hyperlink r:id="rId24" ref="F5"/>
-    <hyperlink r:id="rId25" ref="G5"/>
-    <hyperlink r:id="rId26" ref="I5"/>
-    <hyperlink r:id="rId27" ref="M5"/>
-    <hyperlink r:id="rId28" ref="C6"/>
-    <hyperlink r:id="rId29" ref="E6"/>
-    <hyperlink r:id="rId30" ref="F6"/>
-    <hyperlink r:id="rId31" ref="G6"/>
-    <hyperlink r:id="rId32" ref="I6"/>
-    <hyperlink r:id="rId33" ref="M6"/>
-    <hyperlink r:id="rId34" ref="C7"/>
-    <hyperlink r:id="rId35" ref="E7"/>
-    <hyperlink r:id="rId36" ref="F7"/>
-    <hyperlink r:id="rId37" ref="G7"/>
-    <hyperlink r:id="rId38" ref="I7"/>
-    <hyperlink r:id="rId39" ref="L7"/>
-    <hyperlink r:id="rId40" ref="M7"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="M2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6"/>
+    <hyperlink ref="G3" r:id="rId7"/>
+    <hyperlink ref="I3" r:id="rId8"/>
+    <hyperlink ref="L3" r:id="rId9"/>
+    <hyperlink ref="M3" r:id="rId10"/>
+    <hyperlink ref="C4" r:id="rId11"/>
+    <hyperlink ref="E4" r:id="rId12"/>
+    <hyperlink ref="F4" r:id="rId13"/>
+    <hyperlink ref="G4" r:id="rId14"/>
+    <hyperlink ref="I4" r:id="rId15"/>
+    <hyperlink ref="L4" r:id="rId16"/>
+    <hyperlink ref="M4" r:id="rId17"/>
+    <hyperlink ref="C5" r:id="rId18"/>
+    <hyperlink ref="E5" r:id="rId19"/>
+    <hyperlink ref="F5" r:id="rId20"/>
+    <hyperlink ref="I5" r:id="rId21"/>
+    <hyperlink ref="M5" r:id="rId22"/>
+    <hyperlink ref="C6" r:id="rId23"/>
+    <hyperlink ref="E6" r:id="rId24"/>
+    <hyperlink ref="F6" r:id="rId25"/>
+    <hyperlink ref="G6" r:id="rId26"/>
+    <hyperlink ref="I6" r:id="rId27"/>
+    <hyperlink ref="M6" r:id="rId28"/>
+    <hyperlink ref="C7" r:id="rId29"/>
+    <hyperlink ref="E7" r:id="rId30"/>
+    <hyperlink ref="F7" r:id="rId31"/>
+    <hyperlink ref="G7" r:id="rId32"/>
+    <hyperlink ref="I7" r:id="rId33"/>
+    <hyperlink ref="L7" r:id="rId34"/>
+    <hyperlink ref="M7" r:id="rId35"/>
+    <hyperlink ref="C8" r:id="rId36"/>
+    <hyperlink ref="F8" r:id="rId37"/>
   </hyperlinks>
-  <drawing r:id="rId41"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>